<commit_message>
refactor species_types, start refactoring reactions
</commit_message>
<xml_diff>
--- a/rand_wc_model_gen/model_gen/model_2.xlsx
+++ b/rand_wc_model_gen/model_gen/model_2.xlsx
@@ -41,18 +41,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'dFBA objective species'!$A$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'dFBA objectives'!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Functions!$A$1:$I$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Initial species concentrations'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Initial species concentrations'!$A$1:$L$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Observables!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'Observation sets'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Observations!$A$2:$W$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">References!$A$1:$R$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Species!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Species!$A$1:$J$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'Stop conditions'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Submodels!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Submodels!$A$1:$H$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$24</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4215,7 +4215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="294">
   <si>
     <t>'Model'!A1</t>
   </si>
@@ -4412,7 +4412,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t>2019-08-19 17:26:14</t>
+    <t>2019-08-20 11:04:41</t>
   </si>
   <si>
     <t>Updated</t>
@@ -4433,6 +4433,12 @@
     <t>Evidence</t>
   </si>
   <si>
+    <t>rna_submodel</t>
+  </si>
+  <si>
+    <t>stochastic_simulation_algorithm</t>
+  </si>
+  <si>
     <t>Initial volume</t>
   </si>
   <si>
@@ -4553,6 +4559,15 @@
     <t>C10H12N5O13P3</t>
   </si>
   <si>
+    <t>atp_synthase</t>
+  </si>
+  <si>
+    <t>ATP synthase</t>
+  </si>
+  <si>
+    <t>protein</t>
+  </si>
+  <si>
     <t>cmp</t>
   </si>
   <si>
@@ -4577,6 +4592,12 @@
     <t>C9H12N3O14P3</t>
   </si>
   <si>
+    <t>ctp_synthase</t>
+  </si>
+  <si>
+    <t>CTP synthase</t>
+  </si>
+  <si>
     <t>gmp</t>
   </si>
   <si>
@@ -4601,6 +4622,12 @@
     <t>C10H12N5O14P3</t>
   </si>
   <si>
+    <t>gtp_synthase</t>
+  </si>
+  <si>
+    <t>GTP synthase</t>
+  </si>
+  <si>
     <t>h</t>
   </si>
   <si>
@@ -4631,6 +4658,63 @@
     <t>HO7P2</t>
   </si>
   <si>
+    <t>rna_1</t>
+  </si>
+  <si>
+    <t>RNA 1</t>
+  </si>
+  <si>
+    <t>UACGGUGAUAUGUUC</t>
+  </si>
+  <si>
+    <t>bpforms</t>
+  </si>
+  <si>
+    <t>rna</t>
+  </si>
+  <si>
+    <t>C142H160N53O109P15</t>
+  </si>
+  <si>
+    <t>RNA</t>
+  </si>
+  <si>
+    <t>rna_2</t>
+  </si>
+  <si>
+    <t>RNA 2</t>
+  </si>
+  <si>
+    <t>CAUCCUAUCUUCAUA</t>
+  </si>
+  <si>
+    <t>C139H160N47O108P15</t>
+  </si>
+  <si>
+    <t>rna_3</t>
+  </si>
+  <si>
+    <t>RNA 3</t>
+  </si>
+  <si>
+    <t>GCGAUU</t>
+  </si>
+  <si>
+    <t>C57H65N22O44P6</t>
+  </si>
+  <si>
+    <t>rna_pol</t>
+  </si>
+  <si>
+    <t>RNA polymerase</t>
+  </si>
+  <si>
+    <t>rna_se</t>
+  </si>
+  <si>
+    <t>RNAse</t>
+  </si>
+  <si>
     <t>ump</t>
   </si>
   <si>
@@ -4655,12 +4739,141 @@
     <t>C9H11N2O15P3</t>
   </si>
   <si>
+    <t>utp_synthase</t>
+  </si>
+  <si>
+    <t>UTP synthase</t>
+  </si>
+  <si>
     <t>Species type</t>
   </si>
   <si>
     <t>Compartment</t>
   </si>
   <si>
+    <t>amp[c]</t>
+  </si>
+  <si>
+    <t>molecule</t>
+  </si>
+  <si>
+    <t>atp[c]</t>
+  </si>
+  <si>
+    <t>atp_synthase[c]</t>
+  </si>
+  <si>
+    <t>cmp[c]</t>
+  </si>
+  <si>
+    <t>ctp[c]</t>
+  </si>
+  <si>
+    <t>ctp_synthase[c]</t>
+  </si>
+  <si>
+    <t>gmp[c]</t>
+  </si>
+  <si>
+    <t>gtp[c]</t>
+  </si>
+  <si>
+    <t>gtp_synthase[c]</t>
+  </si>
+  <si>
+    <t>h2o[c]</t>
+  </si>
+  <si>
+    <t>h[c]</t>
+  </si>
+  <si>
+    <t>ppi[c]</t>
+  </si>
+  <si>
+    <t>rna_1[c]</t>
+  </si>
+  <si>
+    <t>rna_2[c]</t>
+  </si>
+  <si>
+    <t>rna_3[c]</t>
+  </si>
+  <si>
+    <t>rna_pol[c]</t>
+  </si>
+  <si>
+    <t>rna_se[c]</t>
+  </si>
+  <si>
+    <t>ump[c]</t>
+  </si>
+  <si>
+    <t>utp[c]</t>
+  </si>
+  <si>
+    <t>utp_synthase[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-amp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-atp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-atp_synthase[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-cmp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ctp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ctp_synthase[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-gmp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-gtp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-gtp_synthase[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-h2o[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-h[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ppi[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-rna_1[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-rna_2[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-rna_3[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-rna_pol[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-rna_se[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ump[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-utp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-utp_synthase[c]</t>
+  </si>
+  <si>
     <t>Expression</t>
   </si>
   <si>
@@ -4691,6 +4904,45 @@
     <t>Maximum</t>
   </si>
   <si>
+    <t>syn_atp</t>
+  </si>
+  <si>
+    <t>synthesis ATP</t>
+  </si>
+  <si>
+    <t>[c]: amp + h + ppi ==&gt; atp + h2o</t>
+  </si>
+  <si>
+    <t>1 / second</t>
+  </si>
+  <si>
+    <t>syn_ctp</t>
+  </si>
+  <si>
+    <t>synthesis CTP</t>
+  </si>
+  <si>
+    <t>[c]: cmp + h + ppi ==&gt; ctp + h2o</t>
+  </si>
+  <si>
+    <t>syn_gtp</t>
+  </si>
+  <si>
+    <t>synthesis GTP</t>
+  </si>
+  <si>
+    <t>[c]: gmp + h + ppi ==&gt; gtp + h2o</t>
+  </si>
+  <si>
+    <t>syn_utp</t>
+  </si>
+  <si>
+    <t>synthesis UTP</t>
+  </si>
+  <si>
+    <t>[c]: h + ppi + ump ==&gt; h2o + utp</t>
+  </si>
+  <si>
     <t>Reaction</t>
   </si>
   <si>
@@ -4722,6 +4974,15 @@
   </si>
   <si>
     <t>gram / liter</t>
+  </si>
+  <si>
+    <t>half_life_rna_1</t>
+  </si>
+  <si>
+    <t>half_life_rna_2</t>
+  </si>
+  <si>
+    <t>half_life_rna_3</t>
   </si>
   <si>
     <t>Genotype</t>
@@ -5274,7 +5535,7 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.01" customHeight="1">
@@ -5292,7 +5553,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.01" customHeight="1">
@@ -5301,7 +5562,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.01" customHeight="1">
@@ -5310,7 +5571,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.01" customHeight="1">
@@ -5337,7 +5598,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.01" customHeight="1">
@@ -5382,7 +5643,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.01" customHeight="1">
@@ -5503,10 +5764,10 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>62</v>
@@ -5575,10 +5836,10 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>62</v>
@@ -5598,14 +5859,14 @@
     </row>
     <row r="2" spans="1:9" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>149</v>
+        <v>220</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>150</v>
+        <v>221</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -5641,7 +5902,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -5662,13 +5923,13 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>151</v>
+        <v>222</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>151</v>
+        <v>222</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>151</v>
+        <v>222</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -5684,25 +5945,25 @@
         <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>153</v>
+        <v>224</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>155</v>
+        <v>226</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>62</v>
@@ -5720,47 +5981,159 @@
         <v>46</v>
       </c>
     </row>
+    <row r="3" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:N2"/>
+  <autoFilter ref="A2:N6"/>
   <mergeCells count="1">
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A3">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A6">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B3">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B6">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C2:C3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C3:C6">
       <formula1>'Submodels'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D2:D3"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E2:E3">
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D3:D6"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E6">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F2:F3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F3:F6">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G2:G3">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G3:G6">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H2:H3">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H3:H6">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I2:I3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I3:I6">
       <formula1>"molar / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J2:J3"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K2:K3"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L2:L3"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M2:M3">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J6"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K6"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L6"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M6">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N2:N3"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N6"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5790,19 +6163,19 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>158</v>
+        <v>242</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>159</v>
+        <v>243</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>62</v>
@@ -5879,19 +6252,19 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>160</v>
+        <v>244</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>161</v>
+        <v>245</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>62</v>
@@ -5968,13 +6341,13 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>162</v>
+        <v>246</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>62</v>
@@ -6048,16 +6421,16 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>163</v>
+        <v>247</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>62</v>
@@ -6113,7 +6486,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6134,16 +6507,16 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>164</v>
+        <v>248</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>62</v>
@@ -6163,7 +6536,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>165</v>
+        <v>249</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6172,7 +6545,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>166</v>
+        <v>250</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -6182,7 +6555,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>167</v>
+        <v>251</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6201,7 +6574,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -6210,7 +6583,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>168</v>
+        <v>252</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6218,35 +6591,92 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
+    <row r="5" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>180</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>180</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>180</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:K4"/>
+  <autoFilter ref="A1:K7"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A4">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A7">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B4">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B7">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C4">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C7">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D4">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D7">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E4">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E7">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F4"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G4"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H4"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I4"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J4">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F7"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G7"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H7"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I7"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J7">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K4"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K7"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6276,10 +6706,10 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>62</v>
@@ -6348,10 +6778,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>169</v>
+        <v>256</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>169</v>
+        <v>256</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>28</v>
@@ -6374,16 +6804,16 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="5" t="s">
-        <v>170</v>
+        <v>257</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>170</v>
+        <v>257</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>171</v>
+        <v>258</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>171</v>
+        <v>258</v>
       </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
@@ -6397,22 +6827,22 @@
         <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>164</v>
+        <v>248</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>172</v>
+        <v>259</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>68</v>
@@ -6421,22 +6851,22 @@
         <v>69</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>173</v>
+        <v>260</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>174</v>
+        <v>261</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>176</v>
+        <v>263</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>177</v>
+        <v>264</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>51</v>
@@ -6766,10 +7196,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>178</v>
+        <v>265</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>178</v>
+        <v>265</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -6786,16 +7216,16 @@
         <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>164</v>
+        <v>248</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>51</v>
@@ -6819,7 +7249,7 @@
         <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>179</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -6892,46 +7322,46 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>267</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>181</v>
+        <v>268</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>269</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>183</v>
+        <v>270</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>184</v>
+        <v>271</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>185</v>
+        <v>272</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>186</v>
+        <v>273</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>187</v>
+        <v>274</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>188</v>
+        <v>275</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>189</v>
+        <v>276</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>190</v>
+        <v>277</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>191</v>
+        <v>278</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>192</v>
+        <v>279</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>62</v>
@@ -7026,28 +7456,28 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>193</v>
+        <v>280</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>194</v>
+        <v>281</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>195</v>
+        <v>282</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>180</v>
+        <v>267</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>196</v>
+        <v>283</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>197</v>
+        <v>284</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>198</v>
+        <v>285</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>199</v>
+        <v>286</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -7127,28 +7557,28 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>200</v>
+        <v>287</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>201</v>
+        <v>288</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>202</v>
+        <v>289</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>203</v>
+        <v>290</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>204</v>
+        <v>291</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>205</v>
+        <v>292</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>206</v>
+        <v>293</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -7169,7 +7599,7 @@
         <v>47</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>179</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -7369,7 +7799,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7408,27 +7838,41 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2" spans="1:8" ht="15.01" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:H1"/>
+  <autoFilter ref="A1:H2"/>
   <dataValidations count="8">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A1:A2">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B1:B2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Framework" error="Value must be a comma-separated list of WC ontology terms &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." promptTitle="Framework" prompt="Enter a comma-separated list of WC ontology terms &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." sqref="C1:C2">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Framework" error="Value must be a comma-separated list of WC ontology terms &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." promptTitle="Framework" prompt="Enter a comma-separated list of WC ontology terms &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." sqref="C2">
       <formula1>"dynamic_flux_balance_analysis,ordinary_differential_equations,stochastic_simulation_algorithm"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="D1:D2"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="E1:E2"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="F1:F2"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="G1:G2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="D2"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="E2"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="F2"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="G2">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="H1:H2"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="H2"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7459,29 +7903,29 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L1" s="4"/>
       <c r="M1" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -7497,46 +7941,46 @@
         <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>62</v>
@@ -7556,26 +8000,26 @@
     </row>
     <row r="3" spans="1:21" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I3" s="3">
         <v>5e-17</v>
@@ -7584,13 +8028,13 @@
         <v>0</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="N3" s="3">
         <v>7.75</v>
@@ -7599,7 +8043,7 @@
         <v>7.75</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -7676,7 +8120,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -7693,22 +8137,22 @@
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -7725,25 +8169,25 @@
         <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>62</v>
@@ -7763,20 +8207,20 @@
     </row>
     <row r="3" spans="1:14" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G3" s="3">
         <v>345.207761998</v>
@@ -7785,7 +8229,7 @@
         <v>-2</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -7795,20 +8239,20 @@
     </row>
     <row r="4" spans="1:14" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G4" s="3">
         <v>503.149285994</v>
@@ -7817,7 +8261,7 @@
         <v>-4</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -7827,29 +8271,19 @@
     </row>
     <row r="5" spans="1:14" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G5" s="3">
-        <v>321.181761998</v>
-      </c>
-      <c r="H5" s="3">
-        <v>-2</v>
-      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -7859,29 +8293,29 @@
     </row>
     <row r="6" spans="1:14" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G6" s="3">
-        <v>479.123285994</v>
+        <v>321.181761998</v>
       </c>
       <c r="H6" s="3">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -7891,29 +8325,29 @@
     </row>
     <row r="7" spans="1:14" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G7" s="3">
-        <v>361.206761998</v>
+        <v>479.123285994</v>
       </c>
       <c r="H7" s="3">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -7923,29 +8357,19 @@
     </row>
     <row r="8" spans="1:14" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="3">
-        <v>519.1482859939999</v>
-      </c>
-      <c r="H8" s="3">
-        <v>-4</v>
-      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -7955,29 +8379,29 @@
     </row>
     <row r="9" spans="1:14" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G9" s="3">
-        <v>1.008</v>
+        <v>361.206761998</v>
       </c>
       <c r="H9" s="3">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -7996,20 +8420,20 @@
         <v>133</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G10" s="3">
-        <v>18.015</v>
+        <v>519.1482859939999</v>
       </c>
       <c r="H10" s="3">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -8019,29 +8443,19 @@
     </row>
     <row r="11" spans="1:14" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C11" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" s="3">
-        <v>174.948523996</v>
-      </c>
-      <c r="H11" s="3">
-        <v>-3</v>
-      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -8051,29 +8465,29 @@
     </row>
     <row r="12" spans="1:14" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G12" s="3">
-        <v>322.165761998</v>
+        <v>1.008</v>
       </c>
       <c r="H12" s="3">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -8083,29 +8497,29 @@
     </row>
     <row r="13" spans="1:14" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G13" s="3">
-        <v>480.1072859940001</v>
+        <v>18.015</v>
       </c>
       <c r="H13" s="3">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -8113,45 +8527,309 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
+    <row r="14" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="3">
+        <v>174.948523996</v>
+      </c>
+      <c r="H14" s="3">
+        <v>-3</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G15" s="3">
+        <v>4817.710429969999</v>
+      </c>
+      <c r="H15" s="3">
+        <v>-16</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="3">
+        <v>4681.63642997</v>
+      </c>
+      <c r="H16" s="3">
+        <v>-16</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1948.099571988</v>
+      </c>
+      <c r="H17" s="3">
+        <v>-7</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G20" s="3">
+        <v>322.165761998</v>
+      </c>
+      <c r="H20" s="3">
+        <v>-2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G21" s="3">
+        <v>480.1072859940001</v>
+      </c>
+      <c r="H21" s="3">
+        <v>-4</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:N13"/>
+  <autoFilter ref="A2:N22"/>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A13">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A22">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B13">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B22">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Value" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="C3:C13">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Value" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="C3:C22">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Format" error="Value must be one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." promptTitle="Format" prompt="Select one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." sqref="D3:D13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Format" error="Value must be one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." promptTitle="Format" prompt="Select one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." sqref="D3:D22">
       <formula1>"smiles,bpforms"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alphabet" error="Value must be one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." promptTitle="Alphabet" prompt="Select one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." sqref="E3:E13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alphabet" error="Value must be one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." promptTitle="Alphabet" prompt="Select one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." sqref="E3:E22">
       <formula1>"dna,rna,protein,canonical_dna,canonical_rna,canonical_protein"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Empirical formula" error="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Value must be an empirical formula (e.g. &quot;H2O&quot;)." promptTitle="Empirical formula" prompt="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Enter an empirical formula (e.g. &quot;H2O&quot;)." sqref="F3:F13"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Molecular weight" error="Value must be a float or blank." promptTitle="Molecular weight" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="G3:G13">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Empirical formula" error="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Value must be an empirical formula (e.g. &quot;H2O&quot;)." promptTitle="Empirical formula" prompt="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Enter an empirical formula (e.g. &quot;H2O&quot;)." sqref="F3:F22"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Molecular weight" error="Value must be a float or blank." promptTitle="Molecular weight" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="G3:G22">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Charge" error="Value must be an integer." promptTitle="Charge" prompt="Enter an integer." sqref="H3:H13">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Charge" error="Value must be an integer." promptTitle="Charge" prompt="Enter an integer." sqref="H3:H22">
       <formula1>-32768</formula1>
       <formula2>32767</formula2>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;I ..." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;Ion&quot;, &quot;am ..." sqref="I3:I13"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J13"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K13"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L13"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M13">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;I ..." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;Ion&quot;, &quot;am ..." sqref="I3:I22"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J22"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K22"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L22"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M22">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N13"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N22"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8160,7 +8838,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8181,13 +8859,13 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>62</v>
@@ -8205,32 +8883,432 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A1:J21"/>
   <dataValidations count="10">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A1:A2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A21">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B1:B2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B21">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Species type" error="Value must be a value from &quot;Species types:A&quot;." promptTitle="Species type" prompt="Select a value from &quot;Species types:A&quot;." sqref="C1:C2">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Species type" error="Value must be a value from &quot;Species types:A&quot;." promptTitle="Species type" prompt="Select a value from &quot;Species types:A&quot;." sqref="C2:C21">
       <formula1>'Species types'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Compartment" error="Value must be a value from &quot;Compartments:A&quot;." promptTitle="Compartment" prompt="Select a value from &quot;Compartments:A&quot;." sqref="D1:D2">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Compartment" error="Value must be a value from &quot;Compartments:A&quot;." promptTitle="Compartment" prompt="Select a value from &quot;Compartments:A&quot;." sqref="D2:D21">
       <formula1>'Compartments'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot; or blank." sqref="E1:E2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot; or blank." sqref="E2:E21">
       <formula1>"molecule"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="F1:F2"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="G1:G2"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="H1:H2"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="I1:I2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="F2:F21"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="G2:G21"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="H2:H21"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="I2:I21">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="J1:J2"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="J2:J21"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8239,7 +9317,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8263,16 +9341,16 @@
         <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>62</v>
@@ -8290,36 +9368,516 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1656088735.675</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1505.53521425</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1505.53521425</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="3">
+        <v>100</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="3">
+        <v>100</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:L21"/>
   <dataValidations count="12">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A1:A2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A21">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B1:B2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B21">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Species" error="Value must be a value from &quot;Species:A&quot;." promptTitle="Species" prompt="Select a value from &quot;Species:A&quot;." sqref="C1:C2">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Species" error="Value must be a value from &quot;Species:A&quot;." promptTitle="Species" prompt="Select a value from &quot;Species:A&quot;." sqref="C2:C21">
       <formula1>'Species'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D1:D2"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E1:E2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D2:D21"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E21">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="F1:F2">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="F2:F21">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G1:G2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G2:G21">
       <formula1>"molecule,molar,millimolar,micromolar,nanomolar,picomolar,femtomolar,attomolar"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H1:H2"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I1:I2"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J1:J2"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K1:K2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H21"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I21"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J21"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K21">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L1:L2"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L21"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
refactor ntp synthesis reactions and rate laws
</commit_message>
<xml_diff>
--- a/rand_wc_model_gen/model_gen/model_2.xlsx
+++ b/rand_wc_model_gen/model_gen/model_2.xlsx
@@ -45,8 +45,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Observables!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'Observation sets'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Observations!$A$2:$W$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">References!$A$1:$R$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$22</definedName>
@@ -4215,7 +4215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="318">
   <si>
     <t>'Model'!A1</t>
   </si>
@@ -4412,7 +4412,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t>2019-08-20 11:04:41</t>
+    <t>2019-08-20 15:45:20</t>
   </si>
   <si>
     <t>Updated</t>
@@ -4664,7 +4664,7 @@
     <t>RNA 1</t>
   </si>
   <si>
-    <t>UACGGUGAUAUGUUC</t>
+    <t>CUGCUG</t>
   </si>
   <si>
     <t>bpforms</t>
@@ -4673,7 +4673,7 @@
     <t>rna</t>
   </si>
   <si>
-    <t>C142H160N53O109P15</t>
+    <t>C56H65N20O45P6</t>
   </si>
   <si>
     <t>RNA</t>
@@ -4685,10 +4685,10 @@
     <t>RNA 2</t>
   </si>
   <si>
-    <t>CAUCCUAUCUUCAUA</t>
-  </si>
-  <si>
-    <t>C139H160N47O108P15</t>
+    <t>GGCGUCAGUGCAUCUACCCACGCGGUG</t>
+  </si>
+  <si>
+    <t>C256H293N102O191P27</t>
   </si>
   <si>
     <t>rna_3</t>
@@ -4697,10 +4697,10 @@
     <t>RNA 3</t>
   </si>
   <si>
-    <t>GCGAUU</t>
-  </si>
-  <si>
-    <t>C57H65N22O44P6</t>
+    <t>AGAUAAGGCUCGGGACGGUAGCGACAC</t>
+  </si>
+  <si>
+    <t>C261H295N114O185P27</t>
   </si>
   <si>
     <t>rna_pol</t>
@@ -4949,6 +4949,33 @@
     <t>Direction</t>
   </si>
   <si>
+    <t>syn_atp-forward</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>kcat_syn_atp* (amp[c] / (km_syn_atp_amp * Avogadro * volume_c + amp[c])) * (ppi[c] / (km_syn_atp_ppi * Avogadro * volume_c + ppi[c]))</t>
+  </si>
+  <si>
+    <t>syn_ctp-forward</t>
+  </si>
+  <si>
+    <t>kcat_syn_ctp* (cmp[c] / (km_syn_ctp_cmp * Avogadro * volume_c + cmp[c])) * (ppi[c] / (km_syn_ctp_ppi * Avogadro * volume_c + ppi[c]))</t>
+  </si>
+  <si>
+    <t>syn_gtp-forward</t>
+  </si>
+  <si>
+    <t>kcat_syn_gtp* (gmp[c] / (km_syn_gtp_gmp * Avogadro * volume_c + gmp[c])) * (ppi[c] / (km_syn_gtp_ppi * Avogadro * volume_c + ppi[c]))</t>
+  </si>
+  <si>
+    <t>syn_utp-forward</t>
+  </si>
+  <si>
+    <t>kcat_syn_utp* (ump[c] / (km_syn_utp_ump * Avogadro * volume_c + ump[c])) * (ppi[c] / (km_syn_utp_ppi * Avogadro * volume_c + ppi[c]))</t>
+  </si>
+  <si>
     <t>Reaction rate units</t>
   </si>
   <si>
@@ -4983,6 +5010,51 @@
   </si>
   <si>
     <t>half_life_rna_3</t>
+  </si>
+  <si>
+    <t>kcat_syn_atp</t>
+  </si>
+  <si>
+    <t>k_cat</t>
+  </si>
+  <si>
+    <t>kcat_syn_ctp</t>
+  </si>
+  <si>
+    <t>kcat_syn_gtp</t>
+  </si>
+  <si>
+    <t>kcat_syn_utp</t>
+  </si>
+  <si>
+    <t>km_syn_atp_amp</t>
+  </si>
+  <si>
+    <t>K_m</t>
+  </si>
+  <si>
+    <t>molar</t>
+  </si>
+  <si>
+    <t>km_syn_atp_ppi</t>
+  </si>
+  <si>
+    <t>km_syn_ctp_cmp</t>
+  </si>
+  <si>
+    <t>km_syn_ctp_ppi</t>
+  </si>
+  <si>
+    <t>km_syn_gtp_gmp</t>
+  </si>
+  <si>
+    <t>km_syn_gtp_ppi</t>
+  </si>
+  <si>
+    <t>km_syn_utp_ppi</t>
+  </si>
+  <si>
+    <t>km_syn_utp_ump</t>
   </si>
   <si>
     <t>Genotype</t>
@@ -5607,7 +5679,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.01" customHeight="1">
@@ -5643,7 +5715,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.01" customHeight="1">
@@ -6142,7 +6214,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6193,36 +6265,132 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:L5"/>
   <dataValidations count="12">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A1:A2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A5">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B1:B2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B5">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C1:C2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C2:C5">
       <formula1>'Reactions'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D1:D2">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D2:D5">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E1:E2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E2:E5">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F1:F2"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G1:G2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F2:F5"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G2:G5">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H1:H2"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I1:I2"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J1:J2"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K1:K2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H5"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I5"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J5"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K5">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L1:L2"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L5"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6261,10 +6429,10 @@
         <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>62</v>
@@ -6347,7 +6515,7 @@
         <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>62</v>
@@ -6421,7 +6589,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>32</v>
@@ -6486,7 +6654,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6513,7 +6681,7 @@
         <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>84</v>
@@ -6536,7 +6704,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6545,7 +6713,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -6555,7 +6723,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6583,7 +6751,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6593,7 +6761,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6612,7 +6780,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6631,7 +6799,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6648,35 +6816,287 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
+    <row r="8" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.003080654</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.003080654</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.003080654</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.003080654</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:K7"/>
+  <autoFilter ref="A1:K19"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A7">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A19">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B7">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B19">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C7">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C19">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D7">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D19">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E7">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E19">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F7"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G7"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H7"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I7"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J7">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F19"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G19"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H19"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I19"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J19">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K7"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K19"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6778,10 +7198,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>28</v>
@@ -6804,16 +7224,16 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="5" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
@@ -6830,7 +7250,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -6842,7 +7262,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>68</v>
@@ -6854,19 +7274,19 @@
         <v>75</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>51</v>
@@ -7196,10 +7616,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -7219,7 +7639,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -7249,7 +7669,7 @@
         <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -7322,46 +7742,46 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>271</v>
+        <v>295</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>273</v>
+        <v>297</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>275</v>
+        <v>299</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>62</v>
@@ -7456,28 +7876,28 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -7560,25 +7980,25 @@
         <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>287</v>
+        <v>311</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>290</v>
+        <v>314</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>291</v>
+        <v>315</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>293</v>
+        <v>317</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -7599,7 +8019,7 @@
         <v>47</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -8579,10 +8999,10 @@
         <v>152</v>
       </c>
       <c r="G15" s="3">
-        <v>4817.710429969999</v>
+        <v>1924.073571988</v>
       </c>
       <c r="H15" s="3">
-        <v>-16</v>
+        <v>-7</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>153</v>
@@ -8613,10 +9033,10 @@
         <v>157</v>
       </c>
       <c r="G16" s="3">
-        <v>4681.63642997</v>
+        <v>8690.974573946</v>
       </c>
       <c r="H16" s="3">
-        <v>-16</v>
+        <v>-28</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>153</v>
@@ -8647,10 +9067,10 @@
         <v>161</v>
       </c>
       <c r="G17" s="3">
-        <v>1948.099571988</v>
+        <v>8825.135573946</v>
       </c>
       <c r="H17" s="3">
-        <v>-7</v>
+        <v>-28</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
refactor rna transcription reactions and ratelaws
</commit_message>
<xml_diff>
--- a/rand_wc_model_gen/model_gen/model_2.xlsx
+++ b/rand_wc_model_gen/model_gen/model_2.xlsx
@@ -45,9 +45,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Observables!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'Observation sets'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Observations!$A$2:$W$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">References!$A$1:$R$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Species!$A$1:$J$21</definedName>
@@ -4215,7 +4215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="341">
   <si>
     <t>'Model'!A1</t>
   </si>
@@ -4412,7 +4412,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t>2019-08-20 15:45:20</t>
+    <t>2019-08-21 10:50:22</t>
   </si>
   <si>
     <t>Updated</t>
@@ -4664,7 +4664,7 @@
     <t>RNA 1</t>
   </si>
   <si>
-    <t>CUGCUG</t>
+    <t>GGGGCCGUACCUAUC</t>
   </si>
   <si>
     <t>bpforms</t>
@@ -4673,7 +4673,7 @@
     <t>rna</t>
   </si>
   <si>
-    <t>C56H65N20O45P6</t>
+    <t>C142H163N56O107P15</t>
   </si>
   <si>
     <t>RNA</t>
@@ -4685,10 +4685,10 @@
     <t>RNA 2</t>
   </si>
   <si>
-    <t>GGCGUCAGUGCAUCUACCCACGCGGUG</t>
-  </si>
-  <si>
-    <t>C256H293N102O191P27</t>
+    <t>AACUUCGUUGAUUCC</t>
+  </si>
+  <si>
+    <t>C140H160N49O109P15</t>
   </si>
   <si>
     <t>rna_3</t>
@@ -4697,10 +4697,10 @@
     <t>RNA 3</t>
   </si>
   <si>
-    <t>AGAUAAGGCUCGGGACGGUAGCGACAC</t>
-  </si>
-  <si>
-    <t>C261H295N114O185P27</t>
+    <t>GAUCCC</t>
+  </si>
+  <si>
+    <t>C56H66N21O43P6</t>
   </si>
   <si>
     <t>rna_pol</t>
@@ -4943,6 +4943,33 @@
     <t>[c]: h + ppi + ump ==&gt; h2o + utp</t>
   </si>
   <si>
+    <t>transcription_rna_1</t>
+  </si>
+  <si>
+    <t>transcription RNA 1</t>
+  </si>
+  <si>
+    <t>[c]: (2) atp + (5) ctp + (5) gtp + h2o + (3) utp ==&gt; h + (15) ppi + rna_1</t>
+  </si>
+  <si>
+    <t>transcription_rna_2</t>
+  </si>
+  <si>
+    <t>transcription RNA 2</t>
+  </si>
+  <si>
+    <t>[c]: (3) atp + (4) ctp + (2) gtp + h2o + (6) utp ==&gt; h + (15) ppi + rna_2</t>
+  </si>
+  <si>
+    <t>transcription_rna_3</t>
+  </si>
+  <si>
+    <t>transcription RNA 3</t>
+  </si>
+  <si>
+    <t>[c]: atp + (3) ctp + gtp + h2o + utp ==&gt; h + (6) ppi + rna_3</t>
+  </si>
+  <si>
     <t>Reaction</t>
   </si>
   <si>
@@ -4976,6 +5003,24 @@
     <t>kcat_syn_utp* (ump[c] / (km_syn_utp_ump * Avogadro * volume_c + ump[c])) * (ppi[c] / (km_syn_utp_ppi * Avogadro * volume_c + ppi[c]))</t>
   </si>
   <si>
+    <t>transcription_rna_1-forward</t>
+  </si>
+  <si>
+    <t>k_trans_rna_1 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c])) * rna_pol[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>transcription_rna_2-forward</t>
+  </si>
+  <si>
+    <t>k_trans_rna_2 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c])) * rna_pol[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>transcription_rna_3-forward</t>
+  </si>
+  <si>
+    <t>k_trans_rna_3 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c])) * rna_pol[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
     <t>Reaction rate units</t>
   </si>
   <si>
@@ -5012,12 +5057,24 @@
     <t>half_life_rna_3</t>
   </si>
   <si>
+    <t>k_trans_rna_1</t>
+  </si>
+  <si>
+    <t>k_cat</t>
+  </si>
+  <si>
+    <t>1 / molar / second</t>
+  </si>
+  <si>
+    <t>k_trans_rna_2</t>
+  </si>
+  <si>
+    <t>k_trans_rna_3</t>
+  </si>
+  <si>
     <t>kcat_syn_atp</t>
   </si>
   <si>
-    <t>k_cat</t>
-  </si>
-  <si>
     <t>kcat_syn_ctp</t>
   </si>
   <si>
@@ -5027,15 +5084,24 @@
     <t>kcat_syn_utp</t>
   </si>
   <si>
+    <t>km_atp_trans</t>
+  </si>
+  <si>
+    <t>K_m</t>
+  </si>
+  <si>
+    <t>molar</t>
+  </si>
+  <si>
+    <t>km_ctp_trans</t>
+  </si>
+  <si>
+    <t>km_gtp_trans</t>
+  </si>
+  <si>
     <t>km_syn_atp_amp</t>
   </si>
   <si>
-    <t>K_m</t>
-  </si>
-  <si>
-    <t>molar</t>
-  </si>
-  <si>
     <t>km_syn_atp_ppi</t>
   </si>
   <si>
@@ -5055,6 +5121,9 @@
   </si>
   <si>
     <t>km_syn_utp_ump</t>
+  </si>
+  <si>
+    <t>km_utp_trans</t>
   </si>
   <si>
     <t>Genotype</t>
@@ -5670,7 +5739,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.01" customHeight="1">
@@ -5679,7 +5748,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.01" customHeight="1">
@@ -5715,7 +5784,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.01" customHeight="1">
@@ -5974,7 +6043,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -6165,47 +6234,131 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
+    <row r="7" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:N6"/>
+  <autoFilter ref="A2:N9"/>
   <mergeCells count="1">
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A6">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A9">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B6">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B9">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C3:C6">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C3:C9">
       <formula1>'Submodels'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D3:D6"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E6">
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D3:D9"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E9">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F3:F6">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F3:F9">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G3:G6">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G3:G9">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H3:H6">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H3:H9">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I3:I6">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I3:I9">
       <formula1>"molar / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J6"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K6"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L6"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M6">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J9"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K9"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L9"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M9">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N6"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N9"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6214,7 +6367,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6235,10 +6388,10 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>103</v>
@@ -6267,18 +6420,18 @@
     </row>
     <row r="2" spans="1:12" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>229</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>232</v>
@@ -6291,18 +6444,18 @@
     </row>
     <row r="3" spans="1:12" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>233</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>232</v>
@@ -6315,18 +6468,18 @@
     </row>
     <row r="4" spans="1:12" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
         <v>236</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>232</v>
@@ -6339,18 +6492,18 @@
     </row>
     <row r="5" spans="1:12" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>239</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>232</v>
@@ -6361,36 +6514,108 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
+    <row r="6" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:L5"/>
+  <autoFilter ref="A1:L8"/>
   <dataValidations count="12">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A5">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A8">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B5">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B8">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C2:C5">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C2:C8">
       <formula1>'Reactions'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D2:D5">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D2:D8">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E2:E5">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E2:E8">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F2:F5"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G2:G5">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F2:F8"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G2:G8">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H5"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I5"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J5"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K5">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H8"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I8"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J8"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K8">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L5"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6429,10 +6654,10 @@
         <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>62</v>
@@ -6515,7 +6740,7 @@
         <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>62</v>
@@ -6589,7 +6814,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>32</v>
@@ -6654,7 +6879,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6681,7 +6906,7 @@
         <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>84</v>
@@ -6704,7 +6929,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6713,7 +6938,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -6723,7 +6948,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6751,7 +6976,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6761,7 +6986,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6780,7 +7005,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6799,7 +7024,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6818,18 +7043,18 @@
     </row>
     <row r="8" spans="1:11" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="D8" s="3">
-        <v>0.003080654</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>232</v>
+        <v>282</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -6839,18 +7064,18 @@
     </row>
     <row r="9" spans="1:11" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="D9" s="3">
-        <v>0.003080654</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>232</v>
+        <v>282</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -6860,18 +7085,18 @@
     </row>
     <row r="10" spans="1:11" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="D10" s="3">
-        <v>0.003080654</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>232</v>
+        <v>282</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -6881,11 +7106,11 @@
     </row>
     <row r="11" spans="1:11" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="D11" s="3">
         <v>0.003080654</v>
@@ -6902,18 +7127,18 @@
     </row>
     <row r="12" spans="1:11" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="D12" s="3">
-        <v>0.001</v>
+        <v>0.003080654</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -6923,18 +7148,18 @@
     </row>
     <row r="13" spans="1:11" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="D13" s="3">
-        <v>5e-05</v>
+        <v>0.003080654</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -6944,18 +7169,18 @@
     </row>
     <row r="14" spans="1:11" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="D14" s="3">
-        <v>0.001</v>
+        <v>0.003080654</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -6965,18 +7190,18 @@
     </row>
     <row r="15" spans="1:11" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="D15" s="3">
-        <v>5e-05</v>
+        <v>0.001</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -6986,18 +7211,18 @@
     </row>
     <row r="16" spans="1:11" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="D16" s="3">
         <v>0.001</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -7007,18 +7232,18 @@
     </row>
     <row r="17" spans="1:11" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="D17" s="3">
-        <v>5e-05</v>
+        <v>0.001</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -7028,18 +7253,18 @@
     </row>
     <row r="18" spans="1:11" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="D18" s="3">
-        <v>5e-05</v>
+        <v>0.001</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -7049,18 +7274,18 @@
     </row>
     <row r="19" spans="1:11" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="D19" s="3">
-        <v>0.001</v>
+        <v>5e-05</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -7068,35 +7293,182 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
+    <row r="20" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D21" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D23" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A26" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:K19"/>
+  <autoFilter ref="A1:K26"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A19">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A26">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B19">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B26">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C19">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C26">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D19">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D26">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E19">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E26">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F19"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G19"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H19"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I19"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J19">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F26"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G26"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H26"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I26"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J26">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K19"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K26"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7198,10 +7570,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>28</v>
@@ -7224,16 +7596,16 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="5" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
@@ -7250,7 +7622,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -7262,7 +7634,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>68</v>
@@ -7274,19 +7646,19 @@
         <v>75</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>284</v>
+        <v>307</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>285</v>
+        <v>308</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>51</v>
@@ -7616,10 +7988,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -7639,7 +8011,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -7669,7 +8041,7 @@
         <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -7742,46 +8114,46 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>62</v>
@@ -7876,28 +8248,28 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -7980,25 +8352,25 @@
         <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>315</v>
+        <v>338</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>316</v>
+        <v>339</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>317</v>
+        <v>340</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -8019,7 +8391,7 @@
         <v>47</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -8999,10 +9371,10 @@
         <v>152</v>
       </c>
       <c r="G15" s="3">
-        <v>1924.073571988</v>
+        <v>4830.75742997</v>
       </c>
       <c r="H15" s="3">
-        <v>-7</v>
+        <v>-16</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>153</v>
@@ -9033,10 +9405,10 @@
         <v>157</v>
       </c>
       <c r="G16" s="3">
-        <v>8690.974573946</v>
+        <v>4737.66042997</v>
       </c>
       <c r="H16" s="3">
-        <v>-28</v>
+        <v>-16</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>153</v>
@@ -9067,10 +9439,10 @@
         <v>161</v>
       </c>
       <c r="G17" s="3">
-        <v>8825.135573946</v>
+        <v>1907.090571988</v>
       </c>
       <c r="H17" s="3">
-        <v>-28</v>
+        <v>-7</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
refactor rna degradation reactions and ratelaws
</commit_message>
<xml_diff>
--- a/rand_wc_model_gen/model_gen/model_2.xlsx
+++ b/rand_wc_model_gen/model_gen/model_2.xlsx
@@ -41,16 +41,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'dFBA objective species'!$A$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'dFBA objectives'!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Functions!$A$1:$I$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Initial species concentrations'!$A$1:$L$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Initial species concentrations'!$A$1:$L$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Observables!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'Observation sets'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Observations!$A$2:$W$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$26</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">References!$A$1:$R$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Species!$A$1:$J$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Species!$A$1:$J$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'Stop conditions'!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Submodels!$A$1:$H$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$24</definedName>
@@ -4215,7 +4215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="397">
   <si>
     <t>'Model'!A1</t>
   </si>
@@ -4412,7 +4412,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t>2019-08-21 10:50:22</t>
+    <t>2019-08-21 12:37:12</t>
   </si>
   <si>
     <t>Updated</t>
@@ -4664,7 +4664,7 @@
     <t>RNA 1</t>
   </si>
   <si>
-    <t>GGGGCCGUACCUAUC</t>
+    <t>UAAUCUGAUCCUGUU</t>
   </si>
   <si>
     <t>bpforms</t>
@@ -4673,7 +4673,7 @@
     <t>rna</t>
   </si>
   <si>
-    <t>C142H163N56O107P15</t>
+    <t>C140H159N48O110P15</t>
   </si>
   <si>
     <t>RNA</t>
@@ -4685,10 +4685,10 @@
     <t>RNA 2</t>
   </si>
   <si>
-    <t>AACUUCGUUGAUUCC</t>
-  </si>
-  <si>
-    <t>C140H160N49O109P15</t>
+    <t>GUUCGCACGUAA</t>
+  </si>
+  <si>
+    <t>C114H130N45O85P12</t>
   </si>
   <si>
     <t>rna_3</t>
@@ -4697,10 +4697,34 @@
     <t>RNA 3</t>
   </si>
   <si>
-    <t>GAUCCC</t>
-  </si>
-  <si>
-    <t>C56H66N21O43P6</t>
+    <t>AACGAAACAACACUUCUC</t>
+  </si>
+  <si>
+    <t>C171H196N69O122P18</t>
+  </si>
+  <si>
+    <t>rna_4</t>
+  </si>
+  <si>
+    <t>RNA 4</t>
+  </si>
+  <si>
+    <t>CCCUUACCGUAGAAA</t>
+  </si>
+  <si>
+    <t>C142H163N56O104P15</t>
+  </si>
+  <si>
+    <t>rna_5</t>
+  </si>
+  <si>
+    <t>RNA 5</t>
+  </si>
+  <si>
+    <t>UCUCCCCAAUGCGGU</t>
+  </si>
+  <si>
+    <t>C140H162N51O108P15</t>
   </si>
   <si>
     <t>rna_pol</t>
@@ -4799,6 +4823,12 @@
     <t>rna_3[c]</t>
   </si>
   <si>
+    <t>rna_4[c]</t>
+  </si>
+  <si>
+    <t>rna_5[c]</t>
+  </si>
+  <si>
     <t>rna_pol[c]</t>
   </si>
   <si>
@@ -4859,6 +4889,12 @@
     <t>dist-init-conc-rna_3[c]</t>
   </si>
   <si>
+    <t>dist-init-conc-rna_4[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-rna_5[c]</t>
+  </si>
+  <si>
     <t>dist-init-conc-rna_pol[c]</t>
   </si>
   <si>
@@ -4904,6 +4940,54 @@
     <t>Maximum</t>
   </si>
   <si>
+    <t>degradation_rna_1</t>
+  </si>
+  <si>
+    <t>transcription RNA 1</t>
+  </si>
+  <si>
+    <t>[c]: (14) h2o + rna_1 ==&gt; (3) amp + (3) cmp + (2) gmp + (14) h + (7) ump</t>
+  </si>
+  <si>
+    <t>1 / second</t>
+  </si>
+  <si>
+    <t>degradation_rna_2</t>
+  </si>
+  <si>
+    <t>transcription RNA 2</t>
+  </si>
+  <si>
+    <t>[c]: (11) h2o + rna_2 ==&gt; (3) amp + (3) cmp + (3) gmp + (11) h + (3) ump</t>
+  </si>
+  <si>
+    <t>degradation_rna_3</t>
+  </si>
+  <si>
+    <t>transcription RNA 3</t>
+  </si>
+  <si>
+    <t>[c]: (17) h2o + rna_3 ==&gt; (8) amp + (6) cmp + gmp + (17) h + (3) ump</t>
+  </si>
+  <si>
+    <t>degradation_rna_4</t>
+  </si>
+  <si>
+    <t>transcription RNA 4</t>
+  </si>
+  <si>
+    <t>[c]: (14) h2o + rna_4 ==&gt; (5) amp + (5) cmp + (2) gmp + (14) h + (3) ump</t>
+  </si>
+  <si>
+    <t>degradation_rna_5</t>
+  </si>
+  <si>
+    <t>transcription RNA 5</t>
+  </si>
+  <si>
+    <t>[c]: (14) h2o + rna_5 ==&gt; (2) amp + (6) cmp + (3) gmp + (14) h + (4) ump</t>
+  </si>
+  <si>
     <t>syn_atp</t>
   </si>
   <si>
@@ -4913,9 +4997,6 @@
     <t>[c]: amp + h + ppi ==&gt; atp + h2o</t>
   </si>
   <si>
-    <t>1 / second</t>
-  </si>
-  <si>
     <t>syn_ctp</t>
   </si>
   <si>
@@ -4946,28 +5027,31 @@
     <t>transcription_rna_1</t>
   </si>
   <si>
-    <t>transcription RNA 1</t>
-  </si>
-  <si>
-    <t>[c]: (2) atp + (5) ctp + (5) gtp + h2o + (3) utp ==&gt; h + (15) ppi + rna_1</t>
+    <t>[c]: (3) atp + (3) ctp + (2) gtp + h2o + (7) utp ==&gt; h + (15) ppi + rna_1</t>
   </si>
   <si>
     <t>transcription_rna_2</t>
   </si>
   <si>
-    <t>transcription RNA 2</t>
-  </si>
-  <si>
-    <t>[c]: (3) atp + (4) ctp + (2) gtp + h2o + (6) utp ==&gt; h + (15) ppi + rna_2</t>
+    <t>[c]: (3) atp + (3) ctp + (3) gtp + h2o + (3) utp ==&gt; h + (12) ppi + rna_2</t>
   </si>
   <si>
     <t>transcription_rna_3</t>
   </si>
   <si>
-    <t>transcription RNA 3</t>
-  </si>
-  <si>
-    <t>[c]: atp + (3) ctp + gtp + h2o + utp ==&gt; h + (6) ppi + rna_3</t>
+    <t>[c]: (8) atp + (6) ctp + gtp + h2o + (3) utp ==&gt; h + (18) ppi + rna_3</t>
+  </si>
+  <si>
+    <t>transcription_rna_4</t>
+  </si>
+  <si>
+    <t>[c]: (5) atp + (5) ctp + (2) gtp + h2o + (3) utp ==&gt; h + (15) ppi + rna_4</t>
+  </si>
+  <si>
+    <t>transcription_rna_5</t>
+  </si>
+  <si>
+    <t>[c]: (2) atp + (6) ctp + (3) gtp + h2o + (4) utp ==&gt; h + (15) ppi + rna_5</t>
   </si>
   <si>
     <t>Reaction</t>
@@ -4976,12 +5060,42 @@
     <t>Direction</t>
   </si>
   <si>
+    <t>degradation_rna_1-forward</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>k_deg_rna_1 * rna_1[c] / (km_deg_rna_1 * Avogadro * volume_c + rna_1[c]) * rna_se[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>degradation_rna_2-forward</t>
+  </si>
+  <si>
+    <t>k_deg_rna_2 * rna_2[c] / (km_deg_rna_2 * Avogadro * volume_c + rna_2[c]) * rna_se[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>degradation_rna_3-forward</t>
+  </si>
+  <si>
+    <t>k_deg_rna_3 * rna_3[c] / (km_deg_rna_3 * Avogadro * volume_c + rna_3[c]) * rna_se[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>degradation_rna_4-forward</t>
+  </si>
+  <si>
+    <t>k_deg_rna_4 * rna_4[c] / (km_deg_rna_4 * Avogadro * volume_c + rna_4[c]) * rna_se[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>degradation_rna_5-forward</t>
+  </si>
+  <si>
+    <t>k_deg_rna_5 * rna_5[c] / (km_deg_rna_5 * Avogadro * volume_c + rna_5[c]) * rna_se[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
     <t>syn_atp-forward</t>
   </si>
   <si>
-    <t>forward</t>
-  </si>
-  <si>
     <t>kcat_syn_atp* (amp[c] / (km_syn_atp_amp * Avogadro * volume_c + amp[c])) * (ppi[c] / (km_syn_atp_ppi * Avogadro * volume_c + ppi[c]))</t>
   </si>
   <si>
@@ -5021,6 +5135,18 @@
     <t>k_trans_rna_3 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c])) * rna_pol[c] / (Avogadro * volume_c)</t>
   </si>
   <si>
+    <t>transcription_rna_4-forward</t>
+  </si>
+  <si>
+    <t>k_trans_rna_4 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c])) * rna_pol[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>transcription_rna_5-forward</t>
+  </si>
+  <si>
+    <t>k_trans_rna_5 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c])) * rna_pol[c] / (Avogadro * volume_c)</t>
+  </si>
+  <si>
     <t>Reaction rate units</t>
   </si>
   <si>
@@ -5057,21 +5183,48 @@
     <t>half_life_rna_3</t>
   </si>
   <si>
+    <t>half_life_rna_4</t>
+  </si>
+  <si>
+    <t>half_life_rna_5</t>
+  </si>
+  <si>
+    <t>k_deg_rna_1</t>
+  </si>
+  <si>
+    <t>k_cat</t>
+  </si>
+  <si>
+    <t>1 / molar / second</t>
+  </si>
+  <si>
+    <t>k_deg_rna_2</t>
+  </si>
+  <si>
+    <t>k_deg_rna_3</t>
+  </si>
+  <si>
+    <t>k_deg_rna_4</t>
+  </si>
+  <si>
+    <t>k_deg_rna_5</t>
+  </si>
+  <si>
     <t>k_trans_rna_1</t>
   </si>
   <si>
-    <t>k_cat</t>
-  </si>
-  <si>
-    <t>1 / molar / second</t>
-  </si>
-  <si>
     <t>k_trans_rna_2</t>
   </si>
   <si>
     <t>k_trans_rna_3</t>
   </si>
   <si>
+    <t>k_trans_rna_4</t>
+  </si>
+  <si>
+    <t>k_trans_rna_5</t>
+  </si>
+  <si>
     <t>kcat_syn_atp</t>
   </si>
   <si>
@@ -5094,6 +5247,21 @@
   </si>
   <si>
     <t>km_ctp_trans</t>
+  </si>
+  <si>
+    <t>km_deg_rna_1</t>
+  </si>
+  <si>
+    <t>km_deg_rna_2</t>
+  </si>
+  <si>
+    <t>km_deg_rna_3</t>
+  </si>
+  <si>
+    <t>km_deg_rna_4</t>
+  </si>
+  <si>
+    <t>km_deg_rna_5</t>
   </si>
   <si>
     <t>km_gtp_trans</t>
@@ -5694,7 +5862,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.01" customHeight="1">
@@ -5703,7 +5871,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.01" customHeight="1">
@@ -5712,7 +5880,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.01" customHeight="1">
@@ -5739,7 +5907,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.01" customHeight="1">
@@ -5748,7 +5916,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.01" customHeight="1">
@@ -5784,7 +5952,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.01" customHeight="1">
@@ -5905,7 +6073,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
@@ -5977,7 +6145,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
@@ -6000,11 +6168,11 @@
     </row>
     <row r="2" spans="1:9" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>93</v>
@@ -6043,7 +6211,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -6064,13 +6232,13 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -6086,22 +6254,22 @@
         <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>84</v>
@@ -6124,22 +6292,22 @@
     </row>
     <row r="3" spans="1:14" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -6152,22 +6320,22 @@
     </row>
     <row r="4" spans="1:14" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6180,22 +6348,22 @@
     </row>
     <row r="5" spans="1:14" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6208,22 +6376,22 @@
     </row>
     <row r="6" spans="1:14" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -6236,22 +6404,22 @@
     </row>
     <row r="7" spans="1:14" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -6264,22 +6432,22 @@
     </row>
     <row r="8" spans="1:14" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -6292,22 +6460,22 @@
     </row>
     <row r="9" spans="1:14" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -6318,47 +6486,243 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
+    <row r="10" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:N9"/>
+  <autoFilter ref="A2:N16"/>
   <mergeCells count="1">
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A9">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A16">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B9">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B16">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C3:C9">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C3:C16">
       <formula1>'Submodels'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D3:D9"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E9">
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D3:D16"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E16">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F3:F9">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F3:F16">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G3:G9">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G3:G16">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H3:H9">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H3:H16">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I3:I9">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I3:I16">
       <formula1>"molar / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J9"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K9"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L9"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M9">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J16"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K16"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L16"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M16">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N9"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N16"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6367,7 +6731,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6388,16 +6752,16 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>251</v>
+        <v>279</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>252</v>
+        <v>280</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>84</v>
@@ -6420,21 +6784,21 @@
     </row>
     <row r="2" spans="1:12" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>255</v>
+        <v>283</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -6444,21 +6808,21 @@
     </row>
     <row r="3" spans="1:12" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>257</v>
+        <v>285</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -6468,21 +6832,21 @@
     </row>
     <row r="4" spans="1:12" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>258</v>
+        <v>286</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -6492,21 +6856,21 @@
     </row>
     <row r="5" spans="1:12" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -6516,21 +6880,21 @@
     </row>
     <row r="6" spans="1:12" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -6540,21 +6904,21 @@
     </row>
     <row r="7" spans="1:12" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -6564,21 +6928,21 @@
     </row>
     <row r="8" spans="1:12" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -6586,36 +6950,204 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
+    <row r="9" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:L8"/>
+  <autoFilter ref="A1:L15"/>
   <dataValidations count="12">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A8">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A15">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B8">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B15">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C2:C8">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C2:C15">
       <formula1>'Reactions'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D2:D8">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D2:D15">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E2:E8">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E2:E15">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F2:F8"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G2:G8">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F2:F15"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G2:G15">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H8"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I8"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J8"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K8">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H15"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I15"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J15"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K15">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L8"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L15"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6645,19 +7177,19 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>62</v>
@@ -6734,13 +7266,13 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>270</v>
+        <v>312</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>62</v>
@@ -6814,7 +7346,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>32</v>
@@ -6879,7 +7411,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6906,7 +7438,7 @@
         <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>84</v>
@@ -6929,7 +7461,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>273</v>
+        <v>315</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6938,7 +7470,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -6948,7 +7480,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6976,7 +7508,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6986,7 +7518,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -7005,7 +7537,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -7024,7 +7556,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -7043,18 +7575,16 @@
     </row>
     <row r="8" spans="1:11" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>281</v>
-      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="3">
-        <v>0.03080654135821979</v>
+        <v>180</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>282</v>
+        <v>61</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -7064,18 +7594,16 @@
     </row>
     <row r="9" spans="1:11" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>283</v>
+        <v>323</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
-        <v>281</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <v>0.03080654135821979</v>
+        <v>180</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>282</v>
+        <v>61</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -7085,18 +7613,18 @@
     </row>
     <row r="10" spans="1:11" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>284</v>
+        <v>324</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>281</v>
+        <v>325</v>
       </c>
       <c r="D10" s="3">
-        <v>0.03080654135821979</v>
+        <v>0.003850817669777474</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>282</v>
+        <v>326</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -7106,18 +7634,18 @@
     </row>
     <row r="11" spans="1:11" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>281</v>
+        <v>325</v>
       </c>
       <c r="D11" s="3">
-        <v>0.003080654</v>
+        <v>0.003850817669777474</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>232</v>
+        <v>326</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -7127,18 +7655,18 @@
     </row>
     <row r="12" spans="1:11" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>281</v>
+        <v>325</v>
       </c>
       <c r="D12" s="3">
-        <v>0.003080654</v>
+        <v>0.003850817669777474</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>232</v>
+        <v>326</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -7148,18 +7676,18 @@
     </row>
     <row r="13" spans="1:11" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>287</v>
+        <v>329</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>281</v>
+        <v>325</v>
       </c>
       <c r="D13" s="3">
-        <v>0.003080654</v>
+        <v>0.003850817669777474</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>232</v>
+        <v>326</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -7169,18 +7697,18 @@
     </row>
     <row r="14" spans="1:11" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>281</v>
+        <v>325</v>
       </c>
       <c r="D14" s="3">
-        <v>0.003080654</v>
+        <v>0.003850817669777474</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>232</v>
+        <v>326</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -7190,18 +7718,18 @@
     </row>
     <row r="15" spans="1:11" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>289</v>
+        <v>331</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D15" s="3">
-        <v>0.001</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>291</v>
+        <v>326</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -7211,18 +7739,18 @@
     </row>
     <row r="16" spans="1:11" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>292</v>
+        <v>332</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D16" s="3">
-        <v>0.001</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>291</v>
+        <v>326</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -7232,18 +7760,18 @@
     </row>
     <row r="17" spans="1:11" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>293</v>
+        <v>333</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D17" s="3">
-        <v>0.001</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>291</v>
+        <v>326</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -7253,18 +7781,18 @@
     </row>
     <row r="18" spans="1:11" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>294</v>
+        <v>334</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D18" s="3">
-        <v>0.001</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>291</v>
+        <v>326</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -7274,18 +7802,18 @@
     </row>
     <row r="19" spans="1:11" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>295</v>
+        <v>335</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D19" s="3">
-        <v>5e-05</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>291</v>
+        <v>326</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -7295,18 +7823,18 @@
     </row>
     <row r="20" spans="1:11" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>296</v>
+        <v>336</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D20" s="3">
-        <v>0.001</v>
+        <v>0.003080654</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>291</v>
+        <v>244</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -7316,18 +7844,18 @@
     </row>
     <row r="21" spans="1:11" ht="15.01" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>297</v>
+        <v>337</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D21" s="3">
-        <v>5e-05</v>
+        <v>0.003080654</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>291</v>
+        <v>244</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -7337,18 +7865,18 @@
     </row>
     <row r="22" spans="1:11" ht="15.01" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>298</v>
+        <v>338</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D22" s="3">
-        <v>0.001</v>
+        <v>0.003080654</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>291</v>
+        <v>244</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -7358,18 +7886,18 @@
     </row>
     <row r="23" spans="1:11" ht="15.01" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>299</v>
+        <v>339</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="D23" s="3">
-        <v>5e-05</v>
+        <v>0.003080654</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>291</v>
+        <v>244</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -7379,18 +7907,18 @@
     </row>
     <row r="24" spans="1:11" ht="15.01" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="D24" s="3">
-        <v>5e-05</v>
+        <v>0.001</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -7400,18 +7928,18 @@
     </row>
     <row r="25" spans="1:11" ht="15.01" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>301</v>
+        <v>343</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="D25" s="3">
         <v>0.001</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -7421,18 +7949,18 @@
     </row>
     <row r="26" spans="1:11" ht="15.01" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="D26" s="3">
-        <v>0.001</v>
+        <v>3.321078080854329e-08</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -7440,35 +7968,329 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
+    <row r="27" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3.321078080854329e-08</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3.321078080854329e-08</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D29" s="3">
+        <v>3.321078080854329e-08</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" s="3">
+        <v>3.321078080854329e-08</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D33" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A35" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D35" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A37" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D37" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D38" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A40" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:K26"/>
+  <autoFilter ref="A1:K40"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A26">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A40">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B26">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B40">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C26">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C40">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D26">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D40">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E26">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E40">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F26"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G26"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H26"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I26"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J26">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F40"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G40"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H40"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I40"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J40">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K26"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K40"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7498,7 +8320,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
@@ -7570,10 +8392,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>303</v>
+        <v>359</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>303</v>
+        <v>359</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>28</v>
@@ -7596,16 +8418,16 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="5" t="s">
-        <v>304</v>
+        <v>360</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>304</v>
+        <v>360</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>305</v>
+        <v>361</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>305</v>
+        <v>361</v>
       </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
@@ -7622,7 +8444,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -7634,7 +8456,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>306</v>
+        <v>362</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>68</v>
@@ -7646,19 +8468,19 @@
         <v>75</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>307</v>
+        <v>363</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>308</v>
+        <v>364</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>309</v>
+        <v>365</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>310</v>
+        <v>366</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>311</v>
+        <v>367</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>51</v>
@@ -7988,10 +8810,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>312</v>
+        <v>368</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>312</v>
+        <v>368</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -8011,7 +8833,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -8041,7 +8863,7 @@
         <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>313</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -8114,46 +8936,46 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>314</v>
+        <v>370</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>315</v>
+        <v>371</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>316</v>
+        <v>372</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>317</v>
+        <v>373</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>318</v>
+        <v>374</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>319</v>
+        <v>375</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>320</v>
+        <v>376</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>321</v>
+        <v>377</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>322</v>
+        <v>378</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>323</v>
+        <v>379</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>324</v>
+        <v>380</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>325</v>
+        <v>381</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>326</v>
+        <v>382</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>62</v>
@@ -8248,28 +9070,28 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>327</v>
+        <v>383</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>329</v>
+        <v>385</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>314</v>
+        <v>370</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>330</v>
+        <v>386</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>331</v>
+        <v>387</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>332</v>
+        <v>388</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>333</v>
+        <v>389</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -8352,25 +9174,25 @@
         <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>334</v>
+        <v>390</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>335</v>
+        <v>391</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>336</v>
+        <v>392</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>338</v>
+        <v>394</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>339</v>
+        <v>395</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>340</v>
+        <v>396</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -8391,7 +9213,7 @@
         <v>47</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>313</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -8912,7 +9734,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -9371,7 +10193,7 @@
         <v>152</v>
       </c>
       <c r="G15" s="3">
-        <v>4830.75742997</v>
+        <v>4738.644429970001</v>
       </c>
       <c r="H15" s="3">
         <v>-16</v>
@@ -9405,10 +10227,10 @@
         <v>157</v>
       </c>
       <c r="G16" s="3">
-        <v>4737.66042997</v>
+        <v>3862.209143976</v>
       </c>
       <c r="H16" s="3">
-        <v>-16</v>
+        <v>-13</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>153</v>
@@ -9439,10 +10261,10 @@
         <v>161</v>
       </c>
       <c r="G17" s="3">
-        <v>1907.090571988</v>
+        <v>5727.337715963999</v>
       </c>
       <c r="H17" s="3">
-        <v>-7</v>
+        <v>-19</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>153</v>
@@ -9460,14 +10282,26 @@
       <c r="B18" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="3">
+        <v>4782.76042997</v>
+      </c>
+      <c r="H18" s="3">
+        <v>-16</v>
+      </c>
       <c r="I18" s="3" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -9477,19 +10311,31 @@
     </row>
     <row r="19" spans="1:14" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+        <v>167</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G19" s="3">
+        <v>4751.69142997</v>
+      </c>
+      <c r="H19" s="3">
+        <v>-16</v>
+      </c>
       <c r="I19" s="3" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -9499,29 +10345,19 @@
     </row>
     <row r="20" spans="1:14" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>107</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G20" s="3">
-        <v>322.165761998</v>
-      </c>
-      <c r="H20" s="3">
-        <v>-2</v>
-      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -9531,29 +10367,19 @@
     </row>
     <row r="21" spans="1:14" ht="15.01" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>107</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G21" s="3">
-        <v>480.1072859940001</v>
-      </c>
-      <c r="H21" s="3">
-        <v>-4</v>
-      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -9568,14 +10394,24 @@
       <c r="B22" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G22" s="3">
+        <v>322.165761998</v>
+      </c>
+      <c r="H22" s="3">
+        <v>-2</v>
+      </c>
       <c r="I22" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -9583,45 +10419,99 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
+    <row r="23" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G23" s="3">
+        <v>480.1072859940001</v>
+      </c>
+      <c r="H23" s="3">
+        <v>-4</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:N22"/>
+  <autoFilter ref="A2:N24"/>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A22">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A24">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B22">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B24">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Value" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="C3:C22">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Value" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="C3:C24">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Format" error="Value must be one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." promptTitle="Format" prompt="Select one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." sqref="D3:D22">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Format" error="Value must be one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." promptTitle="Format" prompt="Select one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." sqref="D3:D24">
       <formula1>"smiles,bpforms"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alphabet" error="Value must be one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." promptTitle="Alphabet" prompt="Select one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." sqref="E3:E22">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alphabet" error="Value must be one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." promptTitle="Alphabet" prompt="Select one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." sqref="E3:E24">
       <formula1>"dna,rna,protein,canonical_dna,canonical_rna,canonical_protein"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Empirical formula" error="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Value must be an empirical formula (e.g. &quot;H2O&quot;)." promptTitle="Empirical formula" prompt="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Enter an empirical formula (e.g. &quot;H2O&quot;)." sqref="F3:F22"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Molecular weight" error="Value must be a float or blank." promptTitle="Molecular weight" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="G3:G22">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Empirical formula" error="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Value must be an empirical formula (e.g. &quot;H2O&quot;)." promptTitle="Empirical formula" prompt="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Enter an empirical formula (e.g. &quot;H2O&quot;)." sqref="F3:F24"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Molecular weight" error="Value must be a float or blank." promptTitle="Molecular weight" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="G3:G24">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Charge" error="Value must be an integer." promptTitle="Charge" prompt="Enter an integer." sqref="H3:H22">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Charge" error="Value must be an integer." promptTitle="Charge" prompt="Enter an integer." sqref="H3:H24">
       <formula1>-32768</formula1>
       <formula2>32767</formula2>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;I ..." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;Ion&quot;, &quot;am ..." sqref="I3:I22"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J22"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K22"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L22"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M22">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;I ..." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;Ion&quot;, &quot;am ..." sqref="I3:I24"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J24"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K24"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L24"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M24">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N22"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N24"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9630,7 +10520,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9651,10 +10541,10 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>84</v>
@@ -9677,7 +10567,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
@@ -9687,7 +10577,7 @@
         <v>86</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -9697,7 +10587,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -9707,7 +10597,7 @@
         <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -9717,7 +10607,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
@@ -9727,7 +10617,7 @@
         <v>86</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -9737,7 +10627,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
@@ -9747,7 +10637,7 @@
         <v>86</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -9757,7 +10647,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -9767,7 +10657,7 @@
         <v>86</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -9777,7 +10667,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -9787,7 +10677,7 @@
         <v>86</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -9797,7 +10687,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
@@ -9807,7 +10697,7 @@
         <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -9817,7 +10707,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
@@ -9827,7 +10717,7 @@
         <v>86</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -9837,7 +10727,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
@@ -9847,7 +10737,7 @@
         <v>86</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -9857,7 +10747,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
@@ -9867,7 +10757,7 @@
         <v>86</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -9877,7 +10767,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
@@ -9887,7 +10777,7 @@
         <v>86</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -9897,7 +10787,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
@@ -9907,7 +10797,7 @@
         <v>86</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -9917,7 +10807,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -9927,7 +10817,7 @@
         <v>86</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -9937,7 +10827,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -9947,7 +10837,7 @@
         <v>86</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -9957,7 +10847,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
@@ -9967,7 +10857,7 @@
         <v>86</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -9977,7 +10867,7 @@
     </row>
     <row r="17" spans="1:10" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
@@ -9987,7 +10877,7 @@
         <v>86</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -9997,17 +10887,17 @@
     </row>
     <row r="18" spans="1:10" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -10017,17 +10907,17 @@
     </row>
     <row r="19" spans="1:10" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -10037,17 +10927,17 @@
     </row>
     <row r="20" spans="1:10" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -10057,7 +10947,7 @@
     </row>
     <row r="21" spans="1:10" ht="15.01" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
@@ -10067,7 +10957,7 @@
         <v>86</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -10075,32 +10965,72 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
+    <row r="22" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.01" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:J21"/>
+  <autoFilter ref="A1:J23"/>
   <dataValidations count="10">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A21">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A23">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B21">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B23">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Species type" error="Value must be a value from &quot;Species types:A&quot;." promptTitle="Species type" prompt="Select a value from &quot;Species types:A&quot;." sqref="C2:C21">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Species type" error="Value must be a value from &quot;Species types:A&quot;." promptTitle="Species type" prompt="Select a value from &quot;Species types:A&quot;." sqref="C2:C23">
       <formula1>'Species types'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Compartment" error="Value must be a value from &quot;Compartments:A&quot;." promptTitle="Compartment" prompt="Select a value from &quot;Compartments:A&quot;." sqref="D2:D21">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Compartment" error="Value must be a value from &quot;Compartments:A&quot;." promptTitle="Compartment" prompt="Select a value from &quot;Compartments:A&quot;." sqref="D2:D23">
       <formula1>'Compartments'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot; or blank." sqref="E2:E21">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot; or blank." sqref="E2:E23">
       <formula1>"molecule"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="F2:F21"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="G2:G21"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="H2:H21"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="I2:I21">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="F2:F23"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="G2:G23"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="H2:H23"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="I2:I23">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="J2:J21"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="J2:J23"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -10109,7 +11039,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10162,11 +11092,11 @@
     </row>
     <row r="2" spans="1:12" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>92</v>
@@ -10176,7 +11106,7 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -10186,11 +11116,11 @@
     </row>
     <row r="3" spans="1:12" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>92</v>
@@ -10200,7 +11130,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -10210,11 +11140,11 @@
     </row>
     <row r="4" spans="1:12" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>92</v>
@@ -10224,7 +11154,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -10234,11 +11164,11 @@
     </row>
     <row r="5" spans="1:12" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>92</v>
@@ -10248,7 +11178,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -10258,11 +11188,11 @@
     </row>
     <row r="6" spans="1:12" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>92</v>
@@ -10272,7 +11202,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -10282,11 +11212,11 @@
     </row>
     <row r="7" spans="1:12" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>92</v>
@@ -10296,7 +11226,7 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -10306,11 +11236,11 @@
     </row>
     <row r="8" spans="1:12" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>92</v>
@@ -10320,7 +11250,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -10330,11 +11260,11 @@
     </row>
     <row r="9" spans="1:12" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>92</v>
@@ -10344,7 +11274,7 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -10354,11 +11284,11 @@
     </row>
     <row r="10" spans="1:12" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>92</v>
@@ -10368,7 +11298,7 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -10378,11 +11308,11 @@
     </row>
     <row r="11" spans="1:12" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>92</v>
@@ -10392,7 +11322,7 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -10402,11 +11332,11 @@
     </row>
     <row r="12" spans="1:12" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>92</v>
@@ -10416,7 +11346,7 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -10426,11 +11356,11 @@
     </row>
     <row r="13" spans="1:12" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>92</v>
@@ -10440,7 +11370,7 @@
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -10450,11 +11380,11 @@
     </row>
     <row r="14" spans="1:12" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>92</v>
@@ -10464,7 +11394,7 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -10474,11 +11404,11 @@
     </row>
     <row r="15" spans="1:12" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>92</v>
@@ -10488,7 +11418,7 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -10498,11 +11428,11 @@
     </row>
     <row r="16" spans="1:12" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>92</v>
@@ -10512,7 +11442,7 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -10522,21 +11452,21 @@
     </row>
     <row r="17" spans="1:12" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E17" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -10546,21 +11476,21 @@
     </row>
     <row r="18" spans="1:12" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E18" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -10570,21 +11500,21 @@
     </row>
     <row r="19" spans="1:12" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E19" s="3">
-        <v>30110.704285</v>
+        <v>100</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -10594,21 +11524,21 @@
     </row>
     <row r="20" spans="1:12" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E20" s="3">
-        <v>30110.704285</v>
+        <v>100</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -10618,21 +11548,21 @@
     </row>
     <row r="21" spans="1:12" ht="15.01" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E21" s="3">
-        <v>1000</v>
+        <v>30110.704285</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -10640,36 +11570,84 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
+    <row r="22" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="3">
+        <v>30110.704285</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:L21"/>
+  <autoFilter ref="A1:L23"/>
   <dataValidations count="12">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A21">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A23">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B21">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B23">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Species" error="Value must be a value from &quot;Species:A&quot;." promptTitle="Species" prompt="Select a value from &quot;Species:A&quot;." sqref="C2:C21">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Species" error="Value must be a value from &quot;Species:A&quot;." promptTitle="Species" prompt="Select a value from &quot;Species:A&quot;." sqref="C2:C23">
       <formula1>'Species'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D2:D21"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E21">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D2:D23"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E23">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="F2:F21">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="F2:F23">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G2:G21">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G2:G23">
       <formula1>"molecule,molar,millimolar,micromolar,nanomolar,picomolar,femtomolar,attomolar"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H21"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I21"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J21"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K21">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H23"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I23"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J23"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K23">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L21"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L23"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>